<commit_message>
chanlenge q not done yet
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amerk\Documents\DA13\Excel\lookups-exercise-zia-da-13\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3281CD78-35DC-4479-8E84-9BB223FF8AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1486D45F-DA72-45A5-B2F0-8B5B7132D263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="91">
   <si>
     <t>Department</t>
   </si>
@@ -304,6 +304,9 @@
   </si>
   <si>
     <t>Actual spending amount - budget amount for fiscal year 2019</t>
+  </si>
+  <si>
+    <t>Question 7</t>
   </si>
 </sst>
 </file>
@@ -889,6 +892,933 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$B$83</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Budget</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$B$84:$B$86</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3130600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3652300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3662400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0A3F-42DC-8607-2337D94AF3FB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$C$83</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$C$84:$C$86</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3115157.5599999898</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3589693.2099999902</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3564983.04999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0A3F-42DC-8607-2337D94AF3FB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="639341855"/>
+        <c:axId val="639333695"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="639341855"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="639333695"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="639333695"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="639341855"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A8F344D-9ABD-CF06-EDE0-F2F85E4CFE98}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -1188,8 +2118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="H75" sqref="H75"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4272,6 +5202,9 @@
       <c r="A54" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="F54" s="10" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
@@ -4284,6 +5217,15 @@
         <v>8</v>
       </c>
       <c r="D55" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H55" s="14" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4303,6 +5245,10 @@
         <f>VLOOKUP(A56,$A$2:$P$52,14, FALSE)</f>
         <v>-9181.0800000000163</v>
       </c>
+      <c r="H56" s="9">
+        <f>INDEX($N$2:$N$52,MATCH(A56,$A$2:$A$52,0))</f>
+        <v>-9181.0800000000163</v>
+      </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
@@ -4320,6 +5266,18 @@
         <f t="shared" ref="D57:D61" si="10">VLOOKUP(A57,$A$2:$P$52,14, FALSE)</f>
         <v>-311228.08999999997</v>
       </c>
+      <c r="F57">
+        <f>INDEX($D$2:$D$52, MATCH(A58,$A$2:$A$52,0))</f>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="G57" s="9">
+        <f t="shared" ref="G57:G61" si="11">INDEX($I$2:$I$52,MATCH(A57,$A$2:$A$52,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H57" s="9">
+        <f t="shared" ref="H57:H61" si="12">INDEX($N$2:$N$52,MATCH(A57,$A$2:$A$52,0))</f>
+        <v>-311228.08999999997</v>
+      </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
@@ -4330,13 +5288,21 @@
         <v>-149396.10000000987</v>
       </c>
       <c r="C58">
-        <f t="shared" ref="C58:C61" si="11">VLOOKUP(A58,$A$2:$P$52,9, FALSE)</f>
+        <f t="shared" ref="C58:C61" si="13">VLOOKUP(A58,$A$2:$P$52,9, FALSE)</f>
         <v>-189254.06000000006</v>
       </c>
       <c r="D58" s="9">
         <f t="shared" si="10"/>
         <v>-374962.91000000015</v>
       </c>
+      <c r="G58" s="9">
+        <f t="shared" si="11"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="H58" s="9">
+        <f t="shared" si="12"/>
+        <v>-374962.91000000015</v>
+      </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -4347,13 +5313,25 @@
         <v>-12230.810000000056</v>
       </c>
       <c r="C59">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D59" s="9">
         <f t="shared" si="10"/>
         <v>-72.879999999888241</v>
       </c>
+      <c r="F59">
+        <f t="shared" ref="F57:F62" si="14">INDEX($D$2:$D$52, MATCH(A59,$A$2:$A$52,0))</f>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="G59" s="9">
+        <f t="shared" si="11"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="H59" s="9">
+        <f t="shared" si="12"/>
+        <v>-72.879999999888241</v>
+      </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
@@ -4364,13 +5342,25 @@
         <v>-4950.4699999999721</v>
       </c>
       <c r="C60">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D60" s="9">
         <f t="shared" si="10"/>
         <v>-1724.9000000000233</v>
       </c>
+      <c r="F60">
+        <f t="shared" si="14"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="G60" s="9">
+        <f t="shared" si="11"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="H60" s="9">
+        <f t="shared" si="12"/>
+        <v>-1724.9000000000233</v>
+      </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
@@ -4381,13 +5371,28 @@
         <v>-184239.79000001028</v>
       </c>
       <c r="C61">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D61" s="9">
         <f t="shared" si="10"/>
         <v>-82077.349999999627</v>
       </c>
+      <c r="F61">
+        <f t="shared" si="14"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="G61" s="9">
+        <f t="shared" si="11"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="H61" s="9">
+        <f t="shared" si="12"/>
+        <v>-82077.349999999627</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F62"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
@@ -4407,8 +5412,17 @@
       <c r="D64" s="14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F64" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H64" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>24</v>
       </c>
@@ -4425,97 +5439,97 @@
         <v>-9181.0800000000163</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>25</v>
       </c>
       <c r="B66">
-        <f t="shared" ref="B66:B70" si="12">_xlfn.XLOOKUP(A66,$A$2:$A$52,$D$2:$D$52)</f>
+        <f t="shared" ref="B66:B70" si="15">_xlfn.XLOOKUP(A66,$A$2:$A$52,$D$2:$D$52)</f>
         <v>0</v>
       </c>
       <c r="C66">
-        <f t="shared" ref="C66:C70" si="13">_xlfn.XLOOKUP(A66,$A$2:$A$52,$I$2:$I$52,0)</f>
+        <f t="shared" ref="C66:C70" si="16">_xlfn.XLOOKUP(A66,$A$2:$A$52,$I$2:$I$52,0)</f>
         <v>0</v>
       </c>
       <c r="D66" s="9">
-        <f t="shared" ref="D66:D70" si="14">_xlfn.XLOOKUP(A66,$A$2:$A$52,$N$2:$N$52,0)</f>
+        <f t="shared" ref="D66:D70" si="17">_xlfn.XLOOKUP(A66,$A$2:$A$52,$N$2:$N$52,0)</f>
         <v>-311228.08999999997</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>32</v>
       </c>
       <c r="B67">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D67" s="9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>38</v>
       </c>
       <c r="B68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C68">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D68" s="9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>39</v>
       </c>
       <c r="B69">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C69">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D69" s="9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>55</v>
       </c>
       <c r="B70">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C70">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D70" s="9">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -4528,106 +5542,115 @@
       <c r="D73" s="14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F73" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H73" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>24</v>
       </c>
       <c r="B74">
-        <f>INDEX($D$2:$D$52, MATCH(A74,$A$2:$A$52,0))</f>
+        <f>INDEX($D$2:$D$52, MATCH($A74,$A$2:$A$52,0))</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="C74" s="9">
-        <f>INDEX($H$2:$H$52,MATCH(A74,$A$2:$A$52,0))</f>
-        <v>467907.84000000003</v>
+        <f>INDEX($I$2:$I$52,MATCH($A74,$A$2:$A$52,0))</f>
+        <v>-27292.159999999974</v>
       </c>
       <c r="D74" s="9">
-        <f t="shared" ref="D74:D79" si="15">INDEX($N$2:$N$52,MATCH(A74,$A$2:$A$52,0))</f>
+        <f>INDEX($N$2:$N$52,MATCH($A74,$A$2:$A$52,0))</f>
         <v>-9181.0800000000163</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>25</v>
       </c>
       <c r="B75">
-        <f t="shared" ref="B75:B79" si="16">INDEX($D$2:$D$52, MATCH(A75,$A$2:$A$52,0))</f>
+        <f t="shared" ref="B75:B79" si="18">INDEX($D$2:$D$52, MATCH($A75,$A$2:$A$52,0))</f>
         <v>0</v>
       </c>
       <c r="C75" s="9">
-        <f t="shared" ref="C75:C79" si="17">INDEX($H$2:$H$52,MATCH(A75,$A$2:$A$52,0))</f>
+        <f t="shared" ref="C75:C79" si="19">INDEX($I$2:$I$52,MATCH($A75,$A$2:$A$52,0))</f>
         <v>0</v>
       </c>
       <c r="D75" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="D75:D79" si="20">INDEX($N$2:$N$52,MATCH($A75,$A$2:$A$52,0))</f>
         <v>-311228.08999999997</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>32</v>
       </c>
       <c r="B76">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C76" s="9">
-        <f t="shared" si="17"/>
-        <v>2671745.94</v>
+        <f t="shared" si="19"/>
+        <v>-189254.06000000006</v>
       </c>
       <c r="D76" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>38</v>
       </c>
       <c r="B77">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C77" s="9">
-        <f t="shared" si="17"/>
-        <v>1067214.42</v>
+        <f t="shared" si="19"/>
+        <v>-45485.580000000075</v>
       </c>
       <c r="D77" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>39</v>
       </c>
       <c r="B78">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C78" s="9">
-        <f t="shared" si="17"/>
-        <v>497194.20999999897</v>
+        <f t="shared" si="19"/>
+        <v>-8005.7900000010268</v>
       </c>
       <c r="D78" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>55</v>
       </c>
       <c r="B79">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C79" s="9">
-        <f t="shared" si="17"/>
-        <v>4956043.6699999897</v>
+        <f t="shared" si="19"/>
+        <v>-133456.33000001032</v>
       </c>
       <c r="D79" s="9">
-        <f t="shared" si="15"/>
+        <f t="shared" si="20"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -4655,11 +5678,11 @@
       </c>
       <c r="B84" s="6">
         <f>INDEX($B$2:$B$52,MATCH($B$87,$A$2:$A$52,0))</f>
-        <v>443300</v>
+        <v>3130600</v>
       </c>
       <c r="C84" s="6">
         <f>INDEX($C$2:$C$52, MATCH($B$87,$A$2:$A$52,0))</f>
-        <v>407090.37</v>
+        <v>3115157.5599999898</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -4668,11 +5691,11 @@
       </c>
       <c r="B85" s="6">
         <f>INDEX($G$2:$G$52,MATCH($B$87,$A$2:$A$52,0))</f>
-        <v>495200</v>
+        <v>3652300</v>
       </c>
       <c r="C85" s="6">
         <f>INDEX($H$2:$H$52,MATCH($B$87,$A$2:$A$52,0))</f>
-        <v>467907.84000000003</v>
+        <v>3589693.2099999902</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -4681,16 +5704,16 @@
       </c>
       <c r="B86" s="6">
         <f>INDEX($L$2:$L$52, MATCH($B$87,$A$2:$A$52,0))</f>
-        <v>487500</v>
+        <v>3662400</v>
       </c>
       <c r="C86" s="6">
         <f>INDEX($M$2:$M$52,MATCH($B$87,$A$2:$A$52, 0))</f>
-        <v>478318.92</v>
+        <v>3564983.04999999</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -4825,24 +5848,26 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB99AC6-F6B8-4A26-96BE-D02EE21B4B6C}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4850,77 +5875,86 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="9"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="9"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="9"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="9"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="9"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="9"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="9"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="9"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>89</v>
       </c>
+      <c r="C10" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>